<commit_message>
- solved bug related with species for CWD - solved bug related with sampOrigId missing on sampId - removed Reject function from toolbar and all its dependencies
</commit_message>
<xml_diff>
--- a/target/classes/tablesSchema.xlsx
+++ b/target/classes/tablesSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="20070" windowHeight="3840" tabRatio="690" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="20070" windowHeight="3840" tabRatio="690" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1623" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="475">
   <si>
     <t>Type</t>
   </si>
@@ -1422,18 +1422,6 @@
     <t>Report Status</t>
   </si>
   <si>
-    <t>%type.code|IF((%type.code==CWD),$RELATION{Preferences,cwdExtCont.code},)</t>
-  </si>
-  <si>
-    <t>AND((%type.code==CWD),(RELATION{Preferences,cwdExtCont.code}==Y))</t>
-  </si>
-  <si>
-    <t>IF(OR((%type.code!=CWD),(RELATION{Preferences,cwdExtCont.code}==N)),F32.A0C9B,)</t>
-  </si>
-  <si>
-    <t>IF((%type.code==RGT),F01.A057G,)IF((%type.code==BSE),F01.A057E,)IF(AND((%type.code==CWD),(RELATION{Preferences,cwdExtCont.code}==N)),F01.A056M,)</t>
-  </si>
-  <si>
     <t>RELATION{Preferences,cwdExtCont.code}</t>
   </si>
   <si>
@@ -1443,13 +1431,25 @@
     <t>IF((RELATION{SummarizedInformation,type.code}!=RGT), RELATION{SummarizedInformation,sampId.label}, )</t>
   </si>
   <si>
-    <t>IF(%type.code!=RGT, origSampId=%sampId.label, )</t>
-  </si>
-  <si>
     <t>IF((RELATION{SummarizedInformation,type.code}!=RGT), origSampId=%origSampId.label, )</t>
   </si>
   <si>
     <t>RELATION{Preferences,cwdExtCont.label}</t>
+  </si>
+  <si>
+    <t>%type.code|IF((%type.code==CWD),$%cwdExtCont.label,)</t>
+  </si>
+  <si>
+    <t>IF(OR((%type.code!=CWD),(%cwdExtCont.code==N)),F32.A0C9B,)</t>
+  </si>
+  <si>
+    <t>IF((%type.code==RGT),F01.A057G,)IF((%type.code==BSE),F01.A057E,)IF(AND((%type.code==CWD),(%cwdExtCont.code==N)),F01.A056M,)</t>
+  </si>
+  <si>
+    <t>AND((%type.code==CWD),(%cwdExtCont.code==Y))</t>
+  </si>
+  <si>
+    <t>IF((%type.code!=RGT), origSampId=%sampId.label, )</t>
   </si>
 </sst>
 </file>
@@ -3797,7 +3797,7 @@
   <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="L3" sqref="L3"/>
@@ -4917,11 +4917,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H25" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="O18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J32" sqref="J32"/>
+      <selection pane="bottomRight" activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5264,11 +5264,17 @@
       <c r="J8" s="6" t="s">
         <v>4</v>
       </c>
+      <c r="M8" s="6" t="s">
+        <v>465</v>
+      </c>
       <c r="N8" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="O8" s="6" t="s">
         <v>469</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="Q8" s="6" t="s">
         <v>5</v>
@@ -5525,10 +5531,10 @@
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="6" t="s">
-        <v>466</v>
+        <v>473</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>466</v>
+        <v>473</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>3</v>
@@ -5815,8 +5821,8 @@
       <c r="J25" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="N25" s="6" t="s">
-        <v>472</v>
+      <c r="P25" s="6" t="s">
+        <v>474</v>
       </c>
       <c r="Q25" s="6" t="s">
         <v>9</v>
@@ -6037,10 +6043,13 @@
         <v>398</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
       <c r="M32" s="6" t="s">
-        <v>467</v>
+        <v>471</v>
+      </c>
+      <c r="N32" s="6" t="s">
+        <v>471</v>
       </c>
       <c r="P32"/>
       <c r="Q32" s="6" t="s">
@@ -6085,10 +6094,13 @@
         <v>109</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>468</v>
+        <v>472</v>
+      </c>
+      <c r="N33" s="6" t="s">
+        <v>472</v>
       </c>
       <c r="Q33" s="6" t="s">
         <v>5</v>
@@ -6444,8 +6456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
@@ -6682,10 +6694,10 @@
         <v>4</v>
       </c>
       <c r="I5" s="32" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="J5" s="32" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>398</v>
@@ -7313,10 +7325,10 @@
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="M23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N33" sqref="N33"/>
+      <selection pane="bottomRight" activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7778,7 +7790,7 @@
         <v>4</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="Q12" s="6" t="s">
         <v>5</v>
@@ -8441,7 +8453,7 @@
         <v>4</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="Q33" s="6" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
* Fixed bug related with sampD not set for all default records in Analytical result level * Removed clone record option for sample and analytical level
</commit_message>
<xml_diff>
--- a/target/classes/tablesSchema.xlsx
+++ b/target/classes/tablesSchema.xlsx
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1641" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="475">
   <si>
     <t>Type</t>
   </si>
@@ -1684,7 +1684,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1700,6 +1700,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1784,7 +1790,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1819,6 +1825,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6698,10 +6705,10 @@
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N13" sqref="N13"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7569,10 +7576,10 @@
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="K11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O14" sqref="O14"/>
+      <selection pane="bottomRight" activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8567,6 +8574,9 @@
       </c>
       <c r="J29" s="6" t="s">
         <v>4</v>
+      </c>
+      <c r="M29" s="32" t="s">
+        <v>271</v>
       </c>
       <c r="N29" s="6" t="s">
         <v>271</v>

</xml_diff>

<commit_message>
- Changes made to the Test type, first test type and status heard on the table schema. All of them where recalculating the value after having performed changes into the table letting, in specific cases, the fields empty, - Removed unused selections from the anMethTypesList picklist, - Solved bug for Scrapie record which was showing in the aggregated data level a value only accepted in analytical result level, - other small changes to the tableSchema.
</commit_message>
<xml_diff>
--- a/target/classes/tablesSchema.xlsx
+++ b/target/classes/tablesSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="20490" windowHeight="4200" tabRatio="690" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="2565" windowWidth="20490" windowHeight="4080" tabRatio="690" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -25,6 +25,40 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>SHAHAJ Alban</author>
+  </authors>
+  <commentList>
+    <comment ref="M23" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>SHAHAJ Alban:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+IF((%type.code==RGT),RF-00004629-PAR,RF-00004628-PAR)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>SHAHAJ Alban</author>
@@ -205,7 +239,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="475">
   <si>
     <t>Type</t>
   </si>
@@ -1257,379 +1291,379 @@
     <t>BSE$AT06A</t>
   </si>
   <si>
+    <t>CWD$AT06A</t>
+  </si>
+  <si>
+    <t>BSE$AT08A</t>
+  </si>
+  <si>
+    <t>SCRAPIE$AT08A</t>
+  </si>
+  <si>
+    <t>CWD$AT08A</t>
+  </si>
+  <si>
+    <t>BSE$AT12A</t>
+  </si>
+  <si>
+    <t>SCRAPIE$AT12A</t>
+  </si>
+  <si>
+    <t>CWD$AT12A</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation,type.code}$%anMethType.code</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation,progId.label}|.|ZERO_PADDING({rowId},6)</t>
+  </si>
+  <si>
+    <t>%country.code|END_TRIM(%reportYear.code,2)|END_TRIM(ZERO_PADDING(%reportMonth.code,2),2)</t>
+  </si>
+  <si>
+    <t>RELATION{Report,reportSenderId.label}|IF_NOT_NULL(RELATION{Report,reportVersion.code},.RELATION{Report,reportVersion.code},)</t>
+  </si>
+  <si>
+    <t>Born in the flock</t>
+  </si>
+  <si>
+    <t>Number of Negative Animals</t>
+  </si>
+  <si>
+    <t>Total number of Tested Samples/Animals</t>
+  </si>
+  <si>
+    <t>Executed test</t>
+  </si>
+  <si>
+    <t>IF((%type.code==RGT),,0)</t>
+  </si>
+  <si>
+    <t>(%type.code!=RGT)</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation,progId.label}|.IF_NOT_NULL(RELATION{CasesInformation,animalId.label},A.|RELATION{CasesInformation,animalId.label},S.|RELATION{CasesInformation,sampId.label})</t>
+  </si>
+  <si>
+    <t>(RELATION{SummarizedInformation,type.code}!=RGT)</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(RELATION{SummarizedInformation,tseTargetGroup.code},tseTargetGroup=RELATION{SummarizedInformation,tseTargetGroup.code},)</t>
+  </si>
+  <si>
+    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT),F02.A06AM,F02.A06AL)</t>
+  </si>
+  <si>
+    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT),Brain,Blood)</t>
+  </si>
+  <si>
+    <t>reportYearsList</t>
+  </si>
+  <si>
+    <t>animalYearsList</t>
+  </si>
+  <si>
+    <t>reportPreviousStatus</t>
+  </si>
+  <si>
+    <t>repPreviousStatus</t>
+  </si>
+  <si>
+    <t>DO NOT TOUCH, AUTOMATICALLY FILLED</t>
+  </si>
+  <si>
+    <t>EU legal reference</t>
+  </si>
+  <si>
+    <t>Res ID</t>
+  </si>
+  <si>
+    <t>EU legislation related to the reason for sampling</t>
+  </si>
+  <si>
+    <t>Prog ID</t>
+  </si>
+  <si>
+    <t>progIdSuffix</t>
+  </si>
+  <si>
+    <t>POS</t>
+  </si>
+  <si>
+    <t>AND((%anMethType.code==AT13A),(RELATION{SummarizedInformation,source.code}==F01.A057G))</t>
+  </si>
+  <si>
+    <t>IF(OR((%internalOpType.label==Reject),(%internalOpType.label==Submit)),No,Yes)</t>
+  </si>
+  <si>
+    <t>(RELATION{SummarizedInformation,source.code}==F01.A057G)</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation,source.code}</t>
+  </si>
+  <si>
+    <t>IF((%internalOpType.label!=Insert),RELATION{Report,reportDatasetId.label},)</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>MTX.gender</t>
+  </si>
+  <si>
+    <t>IF((RELATION{SummarizedInformation,type.code}==RGT),SCRAPIE,)</t>
+  </si>
+  <si>
+    <t>N123A</t>
+  </si>
+  <si>
+    <t>sexLists</t>
+  </si>
+  <si>
+    <t>FM</t>
+  </si>
+  <si>
+    <t>(RELATION{SummarizedInformation,type.code}==RGT)</t>
+  </si>
+  <si>
+    <t>%progLegalRef.code|IF_NOT_NULL(RELATION{SummarizedInformation,tseTargetGroup.code},.|RELATION{SummarizedInformation,tseTargetGroup.code},)</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation,progId.label}|IF((RELATION{SummarizedInformation,type.code}!=RGT),.%progIdSuffix.code,)</t>
+  </si>
+  <si>
+    <t>reportLastMessageId</t>
+  </si>
+  <si>
+    <t>reportLastModifyingMessageId</t>
+  </si>
+  <si>
+    <t>DO NOT TOUCH, used with Refresh Status/Display ack</t>
+  </si>
+  <si>
+    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT),RELATION{SummarizedInformation,animage.code},RELATION{CasesInformation,animage.code})</t>
+  </si>
+  <si>
+    <t>IF((RELATION{SummarizedInformation,type.code}==CWD),RELATION{SummarizedInformation,sex.code},RELATION{CasesInformation,sex.code})</t>
+  </si>
+  <si>
+    <t>A04MQ#RELATION{SummarizedInformation,source.code}$RELATION{CasesInformation,part.code}$RELATION{SummarizedInformation,prod.code}|IF_NOT_NULL(%animage.code,$%animage.code,)|IF_NOT_NULL(%sex.code,$%sex.code,)</t>
+  </si>
+  <si>
+    <t>A04MQ#%source.code$%prod.code|IF((%type.code!=RGT),$%animage.code,)|IF_NOT_NULL(%sex.code,$%sex.code,)</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(%PSUId.label,PSUId=%PSUId.label,)</t>
+  </si>
+  <si>
+    <t>PSUId</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(RELATION{CasesInformation,animalId.code},animalId=RELATION{CasesInformation,animalId.code},)|IF_NOT_NULL(RELATION{CasesInformation,herdId.label},$herdId=RELATION{CasesInformation,herdId.label}, )|IF_NOT_NULL(RELATION{CasesInformation,sampHoldingId.label},$sampHoldingId=RELATION{CasesInformation,sampHoldingId.label},)|IF_NOT_NULL(RELATION{SummarizedInformation,PSUId.label},$PSUId=RELATION{SummarizedInformation,PSUId.label},)</t>
+  </si>
+  <si>
+    <t>Sample/case assessment</t>
+  </si>
+  <si>
+    <t>First test type</t>
+  </si>
+  <si>
+    <t>First test</t>
+  </si>
+  <si>
+    <t>Type of the first executed test</t>
+  </si>
+  <si>
+    <t>First executed test</t>
+  </si>
+  <si>
+    <t>sampInfo</t>
+  </si>
+  <si>
+    <t>D.11</t>
+  </si>
+  <si>
+    <t>origSampId</t>
+  </si>
+  <si>
+    <t>sampUnitType</t>
+  </si>
+  <si>
+    <t>C.02</t>
+  </si>
+  <si>
+    <t>G199A</t>
+  </si>
+  <si>
+    <t>H.01</t>
+  </si>
+  <si>
+    <t>anPortSeq</t>
+  </si>
+  <si>
+    <t>Portion</t>
+  </si>
+  <si>
+    <t>Portion of the analyzed sample</t>
+  </si>
+  <si>
+    <t>AND((%sampEventAsses.code!=J051A),(RELATION{SummarizedInformation,type.code}!=RGT))</t>
+  </si>
+  <si>
+    <t>sampEventAsses</t>
+  </si>
+  <si>
+    <t>AND((%sampEventAsses.code!=J051A),(RELATION{SummarizedInformation,prod.code}==F21.A07RV),(RELATION{SummarizedInformation,type.code}!=RGT))</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(RELATION{CasesInformation,tseNationalCaseId.label},tseNationalCaseId=RELATION{CasesInformation,tseNationalCaseId.label}$,)|IF_NOT_NULL(RELATION{CasesInformation,tseIndexCase.code},tseIndexCase=RELATION{CasesInformation,tseIndexCase.code}$,)|IF_NOT_NULL(RELATION{CasesInformation,sampEventAsses.code},sampEventAsses=RELATION{CasesInformation,sampEventAsses.code},)|IF_NOT_NULL(RELATION{CasesInformation,evalCom.label},$com=RELATION{CasesInformation,evalCom.label},)</t>
+  </si>
+  <si>
+    <t>cwdExtCont</t>
+  </si>
+  <si>
+    <t>pref11</t>
+  </si>
+  <si>
+    <t>yesNoLists</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Sex of the animals</t>
+  </si>
+  <si>
+    <t>%type.code|$%anMethType.code</t>
+  </si>
+  <si>
+    <t>(%type.code==SCRAPIE)</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(%statusHerd.code,statusHerd=%statusHerd.code,)</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>IF(OR((%country.code==EE),(%country.code==FI),(%country.code==LV),(%country.code==LT),(%country.code==PL),(%country.code==SE)),Y,ALL)</t>
+  </si>
+  <si>
+    <t>OR((%type.code==CWD),(%type.code==BSEOS))</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(RELATION{CasesInformation,birthCountry.code},birthCountry=RELATION{CasesInformation,birthCountry.code},)|IF_NOT_NULL(RELATION{SummarizedInformation,statusHerd.code},$statusHerd=RELATION{SummarizedInformation,statusHerd.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthInFlockHerd.code},$birthInFlockHerd=RELATION{CasesInformation,birthInFlockHerd.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthYear.code},$birthYear=RELATION{CasesInformation,birthYear.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthMonth.code},$birthMonth=RELATION{CasesInformation,birthMonth.code},)</t>
+  </si>
+  <si>
+    <t>Herd/Flock status</t>
+  </si>
+  <si>
+    <t>Husbandry system</t>
+  </si>
+  <si>
+    <t>Aggregated-Data-(Level-1)</t>
+  </si>
+  <si>
+    <t>Sample-Level-Data-(Level-2)</t>
+  </si>
+  <si>
+    <t>Analytical-Test-Results-(Level-3)</t>
+  </si>
+  <si>
+    <t>Report-Management</t>
+  </si>
+  <si>
+    <t>IF(OR((%type.code==SCRAPIE),(%type.code==BSEOS)),F,)</t>
+  </si>
+  <si>
+    <t>%progId.label|.0</t>
+  </si>
+  <si>
+    <t>%progId.label</t>
+  </si>
+  <si>
+    <t>NEXT(,)</t>
+  </si>
+  <si>
+    <t>Dataset ID</t>
+  </si>
+  <si>
+    <t>Report Status</t>
+  </si>
+  <si>
+    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT), RELATION{SummarizedInformation,sampId.label}, )</t>
+  </si>
+  <si>
+    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT), origSampId=%origSampId.label, )</t>
+  </si>
+  <si>
+    <t>IF((%type.code!=RGT), origSampId=%sampId.label, )</t>
+  </si>
+  <si>
+    <t>(%type.code==RGT)</t>
+  </si>
+  <si>
+    <t>F01.A057G</t>
+  </si>
+  <si>
+    <t>IF((%type.code==RGT),RF-00004629-PAR#allele=%allele1.label$allele=%allele2.label,RF-00004628-PAR)</t>
+  </si>
+  <si>
+    <t>IF((%type.code==RGT),0,)</t>
+  </si>
+  <si>
+    <t>IF(OR((%type.code!=CWD),(RELATION{Preferences,cwdExtCont.code}==N)),F32.A0C9B,)</t>
+  </si>
+  <si>
+    <t>(RELATION{SummarizedInformation,sex.code}==F32.A0C9B)</t>
+  </si>
+  <si>
+    <t>IF((RELATION{SummarizedInformation,sex.code}!=F32.A0C9B),RELATION{SummarizedInformation,sex.code},)</t>
+  </si>
+  <si>
+    <t>IF((%type.code==RGT),F01.A057G,)IF((%type.code==BSE),F01.A057E,)IF(AND((%type.code==CWD),(RELATION{Preferences,cwdExtCont.code}==N)),F01.A056M,)</t>
+  </si>
+  <si>
+    <t>AND((%type.code==CWD),(RELATION{Preferences,cwdExtCont.code}==Y))</t>
+  </si>
+  <si>
+    <t>(%type.code==CWD)</t>
+  </si>
+  <si>
+    <t>IF((%type.code!=RGT),tseTargetGroup=%tseTargetGroup.code$totSamplesTested=%totSamplesTested.label$totSamplesPositive=%totSamplesPositive.label$totSamplesNegative=%totSamplesNegative.label$totSamplesInconclusive=%totSamplesInconclusive.label$totSamplesUnsuitable=%totSamplesUnsuitable.label,totSamplesTested=%totSamplesTested.label)</t>
+  </si>
+  <si>
+    <t>IF((%type.code!=RGT),SUM(%totSamplesPositive.label,%totSamplesNegative.label,%totSamplesInconclusive.label),)</t>
+  </si>
+  <si>
+    <t>PSU id required</t>
+  </si>
+  <si>
+    <t>Flag to include Primary Sample Unit as mandatory field</t>
+  </si>
+  <si>
+    <t>IF((%type.code==RGT),F01.A057G,)IF((%type.code==BSE),F01.A057E,)</t>
+  </si>
+  <si>
+    <t>(%sampEventAsses.code!=J051A)</t>
+  </si>
+  <si>
+    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT),%paramCodeBaseTerm.code,RF-00004629-PAR)</t>
+  </si>
+  <si>
+    <t>IF((%type.code==RGT),AT13A,AT06A)</t>
+  </si>
+  <si>
+    <t>IF((%type.code==SCRAPIE),RELATION{Preferences,defScreeningSCRAPIE.code},)IF((%type.code==CWD),RELATION{Preferences,defScreeningCWD.code},)IF(OR((%type.code==BSE),(%type.code==BSEOS)),RELATION{Preferences,defScreeningBSE.code},)IF((%type.code==RGT),F089A,)</t>
+  </si>
+  <si>
     <t>SCRAPIE$AT06A</t>
   </si>
   <si>
-    <t>CWD$AT06A</t>
-  </si>
-  <si>
-    <t>BSE$AT08A</t>
-  </si>
-  <si>
-    <t>SCRAPIE$AT08A</t>
-  </si>
-  <si>
-    <t>CWD$AT08A</t>
-  </si>
-  <si>
-    <t>BSE$AT12A</t>
-  </si>
-  <si>
-    <t>SCRAPIE$AT12A</t>
-  </si>
-  <si>
-    <t>CWD$AT12A</t>
-  </si>
-  <si>
-    <t>RELATION{SummarizedInformation,type.code}$%anMethType.code</t>
-  </si>
-  <si>
-    <t>RELATION{SummarizedInformation,progId.label}|.|ZERO_PADDING({rowId},6)</t>
-  </si>
-  <si>
-    <t>%country.code|END_TRIM(%reportYear.code,2)|END_TRIM(ZERO_PADDING(%reportMonth.code,2),2)</t>
-  </si>
-  <si>
-    <t>RELATION{Report,reportSenderId.label}|IF_NOT_NULL(RELATION{Report,reportVersion.code},.RELATION{Report,reportVersion.code},)</t>
-  </si>
-  <si>
-    <t>Born in the flock</t>
-  </si>
-  <si>
-    <t>Number of Negative Animals</t>
-  </si>
-  <si>
-    <t>Total number of Tested Samples/Animals</t>
-  </si>
-  <si>
-    <t>Executed test</t>
-  </si>
-  <si>
-    <t>IF((%type.code==RGT),,0)</t>
-  </si>
-  <si>
-    <t>(%type.code!=RGT)</t>
-  </si>
-  <si>
-    <t>RELATION{SummarizedInformation,progId.label}|.IF_NOT_NULL(RELATION{CasesInformation,animalId.label},A.|RELATION{CasesInformation,animalId.label},S.|RELATION{CasesInformation,sampId.label})</t>
-  </si>
-  <si>
-    <t>(RELATION{SummarizedInformation,type.code}!=RGT)</t>
-  </si>
-  <si>
-    <t>IF_NOT_NULL(RELATION{SummarizedInformation,tseTargetGroup.code},tseTargetGroup=RELATION{SummarizedInformation,tseTargetGroup.code},)</t>
-  </si>
-  <si>
-    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT),F02.A06AM,F02.A06AL)</t>
-  </si>
-  <si>
-    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT),Brain,Blood)</t>
-  </si>
-  <si>
-    <t>reportYearsList</t>
-  </si>
-  <si>
-    <t>animalYearsList</t>
-  </si>
-  <si>
-    <t>reportPreviousStatus</t>
-  </si>
-  <si>
-    <t>repPreviousStatus</t>
-  </si>
-  <si>
-    <t>DO NOT TOUCH, AUTOMATICALLY FILLED</t>
-  </si>
-  <si>
-    <t>EU legal reference</t>
-  </si>
-  <si>
-    <t>Res ID</t>
-  </si>
-  <si>
-    <t>EU legislation related to the reason for sampling</t>
-  </si>
-  <si>
-    <t>Prog ID</t>
-  </si>
-  <si>
-    <t>progIdSuffix</t>
-  </si>
-  <si>
-    <t>POS</t>
-  </si>
-  <si>
-    <t>AND((%anMethType.code==AT13A),(RELATION{SummarizedInformation,source.code}==F01.A057G))</t>
-  </si>
-  <si>
-    <t>IF(OR((%internalOpType.label==Reject),(%internalOpType.label==Submit)),No,Yes)</t>
-  </si>
-  <si>
-    <t>(RELATION{SummarizedInformation,source.code}==F01.A057G)</t>
-  </si>
-  <si>
-    <t>RELATION{SummarizedInformation,source.code}</t>
-  </si>
-  <si>
-    <t>IF((%internalOpType.label!=Insert),RELATION{Report,reportDatasetId.label},)</t>
-  </si>
-  <si>
-    <t>sex</t>
-  </si>
-  <si>
-    <t>MTX.gender</t>
-  </si>
-  <si>
-    <t>IF((RELATION{SummarizedInformation,type.code}==RGT),SCRAPIE,)</t>
-  </si>
-  <si>
-    <t>N123A</t>
-  </si>
-  <si>
-    <t>sexLists</t>
-  </si>
-  <si>
-    <t>FM</t>
-  </si>
-  <si>
-    <t>(RELATION{SummarizedInformation,type.code}==RGT)</t>
-  </si>
-  <si>
-    <t>%progLegalRef.code|IF_NOT_NULL(RELATION{SummarizedInformation,tseTargetGroup.code},.|RELATION{SummarizedInformation,tseTargetGroup.code},)</t>
-  </si>
-  <si>
-    <t>RELATION{SummarizedInformation,progId.label}|IF((RELATION{SummarizedInformation,type.code}!=RGT),.%progIdSuffix.code,)</t>
-  </si>
-  <si>
-    <t>reportLastMessageId</t>
-  </si>
-  <si>
-    <t>reportLastModifyingMessageId</t>
-  </si>
-  <si>
-    <t>DO NOT TOUCH, used with Refresh Status/Display ack</t>
-  </si>
-  <si>
-    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT),RELATION{SummarizedInformation,animage.code},RELATION{CasesInformation,animage.code})</t>
-  </si>
-  <si>
-    <t>IF((RELATION{SummarizedInformation,type.code}==CWD),RELATION{SummarizedInformation,sex.code},RELATION{CasesInformation,sex.code})</t>
-  </si>
-  <si>
-    <t>A04MQ#RELATION{SummarizedInformation,source.code}$RELATION{CasesInformation,part.code}$RELATION{SummarizedInformation,prod.code}|IF_NOT_NULL(%animage.code,$%animage.code,)|IF_NOT_NULL(%sex.code,$%sex.code,)</t>
-  </si>
-  <si>
-    <t>A04MQ#%source.code$%prod.code|IF((%type.code!=RGT),$%animage.code,)|IF_NOT_NULL(%sex.code,$%sex.code,)</t>
-  </si>
-  <si>
-    <t>IF_NOT_NULL(%PSUId.label,PSUId=%PSUId.label,)</t>
-  </si>
-  <si>
-    <t>PSUId</t>
-  </si>
-  <si>
-    <t>IF_NOT_NULL(RELATION{CasesInformation,animalId.code},animalId=RELATION{CasesInformation,animalId.code},)|IF_NOT_NULL(RELATION{CasesInformation,herdId.label},$herdId=RELATION{CasesInformation,herdId.label}, )|IF_NOT_NULL(RELATION{CasesInformation,sampHoldingId.label},$sampHoldingId=RELATION{CasesInformation,sampHoldingId.label},)|IF_NOT_NULL(RELATION{SummarizedInformation,PSUId.label},$PSUId=RELATION{SummarizedInformation,PSUId.label},)</t>
-  </si>
-  <si>
-    <t>Sample/case assessment</t>
-  </si>
-  <si>
-    <t>First test type</t>
-  </si>
-  <si>
-    <t>First test</t>
-  </si>
-  <si>
-    <t>Type of the first executed test</t>
-  </si>
-  <si>
-    <t>First executed test</t>
-  </si>
-  <si>
-    <t>sampInfo</t>
-  </si>
-  <si>
-    <t>D.11</t>
-  </si>
-  <si>
-    <t>origSampId</t>
-  </si>
-  <si>
-    <t>sampUnitType</t>
-  </si>
-  <si>
-    <t>C.02</t>
-  </si>
-  <si>
-    <t>G199A</t>
-  </si>
-  <si>
-    <t>H.01</t>
-  </si>
-  <si>
-    <t>anPortSeq</t>
-  </si>
-  <si>
-    <t>Portion</t>
-  </si>
-  <si>
-    <t>Portion of the analyzed sample</t>
-  </si>
-  <si>
-    <t>AND((%sampEventAsses.code!=J051A),(RELATION{SummarizedInformation,type.code}!=RGT))</t>
-  </si>
-  <si>
-    <t>sampEventAsses</t>
-  </si>
-  <si>
-    <t>AND((%sampEventAsses.code!=J051A),(RELATION{SummarizedInformation,prod.code}==F21.A07RV),(RELATION{SummarizedInformation,type.code}!=RGT))</t>
-  </si>
-  <si>
-    <t>IF_NOT_NULL(RELATION{CasesInformation,tseNationalCaseId.label},tseNationalCaseId=RELATION{CasesInformation,tseNationalCaseId.label}$,)|IF_NOT_NULL(RELATION{CasesInformation,tseIndexCase.code},tseIndexCase=RELATION{CasesInformation,tseIndexCase.code}$,)|IF_NOT_NULL(RELATION{CasesInformation,sampEventAsses.code},sampEventAsses=RELATION{CasesInformation,sampEventAsses.code},)|IF_NOT_NULL(RELATION{CasesInformation,evalCom.label},$com=RELATION{CasesInformation,evalCom.label},)</t>
-  </si>
-  <si>
-    <t>cwdExtCont</t>
-  </si>
-  <si>
-    <t>pref11</t>
-  </si>
-  <si>
-    <t>yesNoLists</t>
-  </si>
-  <si>
-    <t>ALL</t>
-  </si>
-  <si>
-    <t>Sex</t>
-  </si>
-  <si>
-    <t>Sex of the animals</t>
-  </si>
-  <si>
-    <t>%type.code|$%anMethType.code</t>
-  </si>
-  <si>
-    <t>(%type.code==SCRAPIE)</t>
-  </si>
-  <si>
-    <t>IF_NOT_NULL(%statusHerd.code,statusHerd=%statusHerd.code,)</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>IF(OR((%country.code==EE),(%country.code==FI),(%country.code==LV),(%country.code==LT),(%country.code==PL),(%country.code==SE)),Y,ALL)</t>
-  </si>
-  <si>
-    <t>OR((%type.code==CWD),(%type.code==BSEOS))</t>
-  </si>
-  <si>
-    <t>IF_NOT_NULL(RELATION{CasesInformation,birthCountry.code},birthCountry=RELATION{CasesInformation,birthCountry.code},)|IF_NOT_NULL(RELATION{SummarizedInformation,statusHerd.code},$statusHerd=RELATION{SummarizedInformation,statusHerd.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthInFlockHerd.code},$birthInFlockHerd=RELATION{CasesInformation,birthInFlockHerd.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthYear.code},$birthYear=RELATION{CasesInformation,birthYear.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthMonth.code},$birthMonth=RELATION{CasesInformation,birthMonth.code},)</t>
-  </si>
-  <si>
-    <t>Herd/Flock status</t>
-  </si>
-  <si>
-    <t>Husbandry system</t>
-  </si>
-  <si>
-    <t>Aggregated-Data-(Level-1)</t>
-  </si>
-  <si>
-    <t>Sample-Level-Data-(Level-2)</t>
-  </si>
-  <si>
-    <t>Analytical-Test-Results-(Level-3)</t>
-  </si>
-  <si>
-    <t>Report-Management</t>
-  </si>
-  <si>
-    <t>IF(OR((%type.code==SCRAPIE),(%type.code==BSEOS)),F,)</t>
-  </si>
-  <si>
-    <t>%progId.label|.0</t>
-  </si>
-  <si>
-    <t>%progId.label</t>
-  </si>
-  <si>
-    <t>NEXT(,)</t>
-  </si>
-  <si>
-    <t>Dataset ID</t>
-  </si>
-  <si>
-    <t>Report Status</t>
-  </si>
-  <si>
-    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT), RELATION{SummarizedInformation,sampId.label}, )</t>
-  </si>
-  <si>
-    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT), origSampId=%origSampId.label, )</t>
-  </si>
-  <si>
-    <t>IF((%type.code!=RGT), origSampId=%sampId.label, )</t>
-  </si>
-  <si>
-    <t>(%type.code==RGT)</t>
-  </si>
-  <si>
-    <t>F01.A057G</t>
-  </si>
-  <si>
-    <t>IF((%type.code==RGT),RF-00004629-PAR,RF-00004628-PAR)</t>
-  </si>
-  <si>
-    <t>IF((%type.code==RGT),RF-00004629-PAR#allele=%allele1.label$allele=%allele2.label,RF-00004628-PAR)</t>
-  </si>
-  <si>
-    <t>IF((%type.code==RGT),0,)</t>
-  </si>
-  <si>
-    <t>IF(OR((%type.code!=CWD),(RELATION{Preferences,cwdExtCont.code}==N)),F32.A0C9B,)</t>
-  </si>
-  <si>
-    <t>(RELATION{SummarizedInformation,sex.code}==F32.A0C9B)</t>
-  </si>
-  <si>
-    <t>IF((RELATION{SummarizedInformation,sex.code}!=F32.A0C9B),RELATION{SummarizedInformation,sex.code},)</t>
-  </si>
-  <si>
-    <t>IF((%type.code==RGT),F01.A057G,)IF((%type.code==BSE),F01.A057E,)IF(AND((%type.code==CWD),(RELATION{Preferences,cwdExtCont.code}==N)),F01.A056M,)</t>
-  </si>
-  <si>
-    <t>AND((%type.code==CWD),(RELATION{Preferences,cwdExtCont.code}==Y))</t>
-  </si>
-  <si>
-    <t>(%type.code==CWD)</t>
-  </si>
-  <si>
-    <t>IF((%type.code==RGT),AT13A,AT06A)</t>
-  </si>
-  <si>
-    <t>IF((%type.code==SCRAPIE),RELATION{Preferences,defScreeningSCRAPIE.code},)IF((%type.code==CWD),RELATION{Preferences,defScreeningCWD.code},)IF(OR((%type.code==BSE),(%type.code==BSEOS)),RELATION{Preferences,defScreeningBSE.code},)IF((%type.code==RGT),F089A,)</t>
-  </si>
-  <si>
-    <t>IF((%type.code!=RGT),tseTargetGroup=%tseTargetGroup.code$totSamplesTested=%totSamplesTested.label$totSamplesPositive=%totSamplesPositive.label$totSamplesNegative=%totSamplesNegative.label$totSamplesInconclusive=%totSamplesInconclusive.label$totSamplesUnsuitable=%totSamplesUnsuitable.label,totSamplesTested=%totSamplesTested.label)</t>
-  </si>
-  <si>
-    <t>IF((%type.code!=RGT),SUM(%totSamplesPositive.label,%totSamplesNegative.label,%totSamplesInconclusive.label),)</t>
-  </si>
-  <si>
-    <t>PSU id required</t>
-  </si>
-  <si>
-    <t>Flag to include Primary Sample Unit as mandatory field</t>
-  </si>
-  <si>
-    <t>IF((%type.code==RGT),F01.A057G,)IF((%type.code==BSE),F01.A057E,)</t>
-  </si>
-  <si>
-    <t>(%sampEventAsses.code!=J051A)</t>
-  </si>
-  <si>
-    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT),%paramCodeBaseTerm.code,RF-00004629-PAR)</t>
+    <t>IF((%type.code==SCRAPIE),BSE,%type.code)</t>
   </si>
 </sst>
 </file>
@@ -1790,7 +1824,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1826,6 +1860,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3998,10 +4033,10 @@
   <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4118,16 +4153,16 @@
     </row>
     <row r="3" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>428</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="F3" s="24" t="s">
         <v>12</v>
@@ -4145,16 +4180,16 @@
         <v>9</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="L3" s="25" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>9</v>
@@ -4236,7 +4271,7 @@
         <v>112</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>350</v>
+        <v>473</v>
       </c>
       <c r="R5" s="2">
         <v>4</v>
@@ -4274,7 +4309,7 @@
         <v>112</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="R6" s="2">
         <v>5</v>
@@ -4312,7 +4347,7 @@
         <v>112</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="R7" s="2">
         <v>6</v>
@@ -4350,7 +4385,7 @@
         <v>112</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="R8" s="2">
         <v>7</v>
@@ -4388,7 +4423,7 @@
         <v>112</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="R9" s="2">
         <v>8</v>
@@ -4427,7 +4462,7 @@
         <v>112</v>
       </c>
       <c r="L10" s="27" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="R10" s="2">
         <v>9</v>
@@ -4466,7 +4501,7 @@
         <v>112</v>
       </c>
       <c r="L11" s="27" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="R11" s="2">
         <v>10</v>
@@ -4505,7 +4540,7 @@
         <v>112</v>
       </c>
       <c r="L12" s="27" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
@@ -4646,7 +4681,7 @@
         <v>9</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="8" t="s">
@@ -4751,7 +4786,7 @@
         <v>300</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>5</v>
@@ -4877,7 +4912,7 @@
       <c r="C8" s="17"/>
       <c r="D8" s="18"/>
       <c r="E8" s="17" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F8" s="17" t="s">
         <v>174</v>
@@ -4908,13 +4943,13 @@
     </row>
     <row r="9" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
       <c r="D9" s="18"/>
       <c r="E9" s="17" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>174</v>
@@ -4945,13 +4980,13 @@
     </row>
     <row r="10" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="18"/>
       <c r="E10" s="17" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>174</v>
@@ -4989,10 +5024,10 @@
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="18" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>174</v>
@@ -5032,10 +5067,10 @@
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="18" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F12" s="17" t="s">
         <v>174</v>
@@ -5068,15 +5103,15 @@
     </row>
     <row r="13" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
+        <v>374</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>375</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>376</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="18"/>
       <c r="E13" s="17" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F13" s="17" t="s">
         <v>174</v>
@@ -5115,14 +5150,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="M14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P10" sqref="P10"/>
+      <selection pane="bottomRight" activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5142,7 +5177,7 @@
     <col min="14" max="14" width="50.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17.42578125" style="6" customWidth="1"/>
     <col min="16" max="16" width="52.5703125" style="6" customWidth="1"/>
-    <col min="17" max="17" width="9.85546875" style="6" customWidth="1"/>
+    <col min="17" max="17" width="20" style="6" customWidth="1"/>
     <col min="18" max="18" width="9.140625" style="6"/>
     <col min="19" max="19" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="9.140625" style="6"/>
@@ -5271,7 +5306,7 @@
         <v>3</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>3</v>
@@ -5283,10 +5318,10 @@
         <v>312</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>5</v>
@@ -5306,7 +5341,7 @@
         <v>57</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>69</v>
@@ -5321,7 +5356,7 @@
         <v>3</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>3</v>
@@ -5365,10 +5400,10 @@
         <v>74</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>3</v>
@@ -5409,10 +5444,10 @@
         <v>18</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>3</v>
@@ -5435,40 +5470,40 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D7" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>431</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>432</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>3</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="L7" s="29" t="s">
         <v>312</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="P7"/>
       <c r="Q7" s="6" t="s">
@@ -5492,10 +5527,10 @@
         <v>89</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>12</v>
@@ -5504,10 +5539,10 @@
         <v>90</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>3</v>
@@ -5515,14 +5550,11 @@
       <c r="K8" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="L8" s="6" t="s">
-        <v>312</v>
+      <c r="L8" s="29" t="s">
+        <v>474</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>466</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="Q8" s="6" t="s">
         <v>9</v>
@@ -5545,10 +5577,10 @@
         <v>92</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>12</v>
@@ -5557,10 +5589,10 @@
         <v>93</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>3</v>
@@ -5569,13 +5601,10 @@
         <v>112</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>467</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
       <c r="Q9" s="6" t="s">
         <v>9</v>
@@ -5595,7 +5624,7 @@
         <v>34</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>36</v>
@@ -5607,10 +5636,10 @@
         <v>37</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>3</v>
@@ -5622,10 +5651,7 @@
         <v>312</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>446</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="Q10" s="6" t="s">
         <v>5</v>
@@ -5639,23 +5665,23 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>202</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>174</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="6" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>3</v>
@@ -5681,7 +5707,7 @@
         <v>25</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F12" s="21" t="s">
         <v>238</v>
@@ -5690,16 +5716,16 @@
         <v>8</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O12" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="Q12" s="6" t="s">
         <v>5</v>
@@ -5728,16 +5754,16 @@
         <v>8</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O13" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="Q13" s="6" t="s">
         <v>5</v>
@@ -5766,16 +5792,16 @@
         <v>8</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J14" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O14" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="Q14" s="6" t="s">
         <v>5</v>
@@ -5795,7 +5821,7 @@
         <v>20</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>238</v>
@@ -5804,19 +5830,19 @@
         <v>8</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O15" s="6" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="P15" s="6" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="Q15" s="6" t="s">
         <v>5</v>
@@ -5845,16 +5871,16 @@
         <v>8</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O16" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="Q16" s="6" t="s">
         <v>5</v>
@@ -5874,7 +5900,7 @@
         <v>7</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F17" s="17" t="s">
         <v>174</v>
@@ -5892,7 +5918,7 @@
         <v>3</v>
       </c>
       <c r="O17" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>9</v>
@@ -5919,10 +5945,10 @@
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>3</v>
@@ -5931,7 +5957,7 @@
         <v>319</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="Q18" s="6" t="s">
         <v>5</v>
@@ -5961,10 +5987,10 @@
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="J19" s="6" t="s">
         <v>3</v>
@@ -5973,7 +5999,7 @@
         <v>319</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="Q19" s="6" t="s">
         <v>5</v>
@@ -6100,14 +6126,9 @@
       <c r="J23" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="M23" s="6" t="s">
-        <v>457</v>
-      </c>
-      <c r="O23" s="6" t="s">
-        <v>457</v>
-      </c>
+      <c r="M23" s="33"/>
       <c r="P23" s="6" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="Q23" s="6" t="s">
         <v>9</v>
@@ -6194,7 +6215,7 @@
         <v>4</v>
       </c>
       <c r="P26" s="6" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="Q26" s="6" t="s">
         <v>9</v>
@@ -6223,7 +6244,7 @@
         <v>4</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Q27" s="6" t="s">
         <v>3</v>
@@ -6345,7 +6366,7 @@
         <v>4</v>
       </c>
       <c r="P31" s="6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="Q31" s="6" t="s">
         <v>9</v>
@@ -6377,7 +6398,7 @@
         <v>4</v>
       </c>
       <c r="P32" s="6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="Q32" s="6" t="s">
         <v>9</v>
@@ -6441,7 +6462,7 @@
         <v>4</v>
       </c>
       <c r="P34" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="Q34" s="6" t="s">
         <v>9</v>
@@ -6473,7 +6494,7 @@
         <v>4</v>
       </c>
       <c r="P35" s="6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="Q35" s="6" t="s">
         <v>9</v>
@@ -6481,13 +6502,13 @@
     </row>
     <row r="36" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>413</v>
       </c>
-      <c r="B36" s="6" t="s">
-        <v>414</v>
-      </c>
       <c r="C36" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>174</v>
@@ -6502,7 +6523,7 @@
         <v>4</v>
       </c>
       <c r="P36" s="6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="Q36" s="6" t="s">
         <v>9</v>
@@ -6569,7 +6590,7 @@
         <v>4</v>
       </c>
       <c r="P38" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="Q38" s="6" t="s">
         <v>9</v>
@@ -6630,7 +6651,7 @@
         <v>4</v>
       </c>
       <c r="P40" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q40" s="6" t="s">
         <v>9</v>
@@ -6694,8 +6715,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -6705,10 +6727,10 @@
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11:XFD11"/>
+      <selection pane="bottomRight" activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6795,13 +6817,13 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B2" t="s">
         <v>191</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>211</v>
@@ -6813,10 +6835,10 @@
         <v>320</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="J2" s="30" t="s">
         <v>3</v>
@@ -6904,10 +6926,10 @@
         <v>303</v>
       </c>
       <c r="M4" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="O4" s="6" t="s">
         <v>371</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>372</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>5</v>
@@ -6921,40 +6943,40 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>431</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>432</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K5" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>393</v>
       </c>
-      <c r="L5" s="6" t="s">
-        <v>394</v>
-      </c>
       <c r="M5" s="6" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="Q5" s="6" t="s">
         <v>5</v>
@@ -6983,10 +7005,10 @@
         <v>74</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="J6" s="30" t="s">
         <v>4</v>
@@ -6995,7 +7017,7 @@
         <v>111</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="Q6" s="6" t="s">
         <v>5</v>
@@ -7024,7 +7046,7 @@
         <v>8</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>3</v>
@@ -7062,7 +7084,7 @@
         <v>8</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>3</v>
@@ -7206,7 +7228,7 @@
         <v>217</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I12" s="17" t="s">
         <v>3</v>
@@ -7247,13 +7269,13 @@
         <v>197</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="I13" s="29" t="s">
         <v>3</v>
       </c>
       <c r="J13" s="30" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>198</v>
@@ -7290,7 +7312,7 @@
         <v>42</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I14" s="17" t="s">
         <v>3</v>
@@ -7330,7 +7352,7 @@
         <v>282</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>3</v>
@@ -7339,7 +7361,7 @@
         <v>3</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="Q15" s="6" t="s">
         <v>5</v>
@@ -7366,7 +7388,7 @@
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I16" s="20" t="s">
         <v>3</v>
@@ -7392,7 +7414,7 @@
         <v>34</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>309</v>
@@ -7413,10 +7435,10 @@
         <v>3</v>
       </c>
       <c r="K17" s="20" t="s">
+        <v>428</v>
+      </c>
+      <c r="L17" s="6" t="s">
         <v>429</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>430</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>5</v>
@@ -7575,11 +7597,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="K11" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="M8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M29" sqref="M29"/>
+      <selection pane="bottomRight" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7676,19 +7698,19 @@
         <v>12</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>319</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="Q2" s="6" t="s">
         <v>5</v>
@@ -7714,19 +7736,19 @@
         <v>12</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>319</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>5</v>
@@ -7767,7 +7789,7 @@
         <v>3</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M4" s="6" t="s">
         <v>294</v>
@@ -7802,7 +7824,7 @@
         <v>4</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q5" s="6" t="s">
         <v>5</v>
@@ -7822,7 +7844,7 @@
         <v>142</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>12</v>
@@ -7843,7 +7865,7 @@
         <v>112</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="Q6" s="6" t="s">
         <v>9</v>
@@ -7936,19 +7958,19 @@
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>420</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>419</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>420</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>421</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>422</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>174</v>
@@ -8015,7 +8037,7 @@
         <v>4</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="Q11" s="6" t="s">
         <v>9</v>
@@ -8023,10 +8045,10 @@
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>174</v>
@@ -8041,7 +8063,7 @@
         <v>4</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="Q12" s="6" t="s">
         <v>5</v>
@@ -8099,7 +8121,7 @@
         <v>4</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="Q14" s="6" t="s">
         <v>5</v>
@@ -8166,7 +8188,7 @@
         <v>4</v>
       </c>
       <c r="P16" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="Q16" s="6" t="s">
         <v>9</v>
@@ -8174,7 +8196,7 @@
     </row>
     <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>174</v>
@@ -8192,7 +8214,7 @@
         <v>4</v>
       </c>
       <c r="P17" s="6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>5</v>
@@ -8224,7 +8246,7 @@
         <v>4</v>
       </c>
       <c r="P18" s="6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="Q18" s="6" t="s">
         <v>9</v>
@@ -8241,10 +8263,10 @@
         <v>11</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>174</v>
@@ -8262,7 +8284,7 @@
         <v>4</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Q19" s="6" t="s">
         <v>9</v>
@@ -8363,7 +8385,7 @@
         <v>95</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>256</v>
@@ -8384,7 +8406,7 @@
         <v>3</v>
       </c>
       <c r="O23" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="Q23" s="6" t="s">
         <v>9</v>
@@ -8419,7 +8441,7 @@
         <v>4</v>
       </c>
       <c r="M24" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="Q24" s="6" t="s">
         <v>9</v>
@@ -8611,7 +8633,7 @@
         <v>4</v>
       </c>
       <c r="P30" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="Q30" s="6" t="s">
         <v>9</v>
@@ -8640,7 +8662,7 @@
         <v>4</v>
       </c>
       <c r="P31" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q31" s="6" t="s">
         <v>9</v>
@@ -8686,13 +8708,13 @@
     </row>
     <row r="33" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>413</v>
       </c>
-      <c r="B33" s="6" t="s">
-        <v>414</v>
-      </c>
       <c r="C33" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>174</v>
@@ -8707,7 +8729,7 @@
         <v>4</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="Q33" s="6" t="s">
         <v>9</v>
@@ -8771,7 +8793,7 @@
         <v>4</v>
       </c>
       <c r="P35" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="Q35" s="6" t="s">
         <v>9</v>
@@ -8867,7 +8889,7 @@
         <v>4</v>
       </c>
       <c r="P38" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q38" s="6" t="s">
         <v>9</v>
@@ -8875,13 +8897,13 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>416</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>417</v>
-      </c>
       <c r="C39" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>174</v>
@@ -8896,13 +8918,13 @@
         <v>4</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="N39" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="O39" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="Q39" s="6" t="s">
         <v>9</v>
@@ -8945,7 +8967,7 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>57</v>
@@ -8963,7 +8985,7 @@
         <v>4</v>
       </c>
       <c r="N41" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="Q41" s="6" t="s">
         <v>5</v>
@@ -9009,7 +9031,7 @@
         <v>342</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="K43" s="6" t="s">
         <v>339</v>
@@ -9213,7 +9235,7 @@
         <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -9221,7 +9243,7 @@
         <v>170</v>
       </c>
       <c r="B3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -9245,7 +9267,7 @@
         <v>221</v>
       </c>
       <c r="B6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -9253,7 +9275,7 @@
         <v>227</v>
       </c>
       <c r="B7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
   </sheetData>
@@ -9617,10 +9639,10 @@
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
       <c r="P10" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
@@ -9676,7 +9698,7 @@
         <v>4</v>
       </c>
       <c r="P12" s="10" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="Q12" s="2" t="s">
         <v>344</v>

</xml_diff>

<commit_message>
Modifications done to the BR TSE48 and TSE49 and other optimisations with the catch clauses.
</commit_message>
<xml_diff>
--- a/target/classes/tablesSchema.xlsx
+++ b/target/classes/tablesSchema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2565" windowWidth="20490" windowHeight="4080" tabRatio="690" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2565" windowWidth="20490" windowHeight="4080" tabRatio="690" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -239,7 +239,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1640" uniqueCount="475">
   <si>
     <t>Type</t>
   </si>
@@ -1264,9 +1264,6 @@
     <t>testAim</t>
   </si>
   <si>
-    <t>RELATION{SummarizedInformation,type.code}|%anMethType.code</t>
-  </si>
-  <si>
     <t>(%anMethType.code!=AT13A)</t>
   </si>
   <si>
@@ -1312,358 +1309,361 @@
     <t>CWD$AT12A</t>
   </si>
   <si>
+    <t>RELATION{SummarizedInformation,progId.label}|.|ZERO_PADDING({rowId},6)</t>
+  </si>
+  <si>
+    <t>%country.code|END_TRIM(%reportYear.code,2)|END_TRIM(ZERO_PADDING(%reportMonth.code,2),2)</t>
+  </si>
+  <si>
+    <t>RELATION{Report,reportSenderId.label}|IF_NOT_NULL(RELATION{Report,reportVersion.code},.RELATION{Report,reportVersion.code},)</t>
+  </si>
+  <si>
+    <t>Born in the flock</t>
+  </si>
+  <si>
+    <t>Number of Negative Animals</t>
+  </si>
+  <si>
+    <t>Total number of Tested Samples/Animals</t>
+  </si>
+  <si>
+    <t>Executed test</t>
+  </si>
+  <si>
+    <t>IF((%type.code==RGT),,0)</t>
+  </si>
+  <si>
+    <t>(%type.code!=RGT)</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation,progId.label}|.IF_NOT_NULL(RELATION{CasesInformation,animalId.label},A.|RELATION{CasesInformation,animalId.label},S.|RELATION{CasesInformation,sampId.label})</t>
+  </si>
+  <si>
+    <t>(RELATION{SummarizedInformation,type.code}!=RGT)</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(RELATION{SummarizedInformation,tseTargetGroup.code},tseTargetGroup=RELATION{SummarizedInformation,tseTargetGroup.code},)</t>
+  </si>
+  <si>
+    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT),F02.A06AM,F02.A06AL)</t>
+  </si>
+  <si>
+    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT),Brain,Blood)</t>
+  </si>
+  <si>
+    <t>reportYearsList</t>
+  </si>
+  <si>
+    <t>animalYearsList</t>
+  </si>
+  <si>
+    <t>reportPreviousStatus</t>
+  </si>
+  <si>
+    <t>repPreviousStatus</t>
+  </si>
+  <si>
+    <t>DO NOT TOUCH, AUTOMATICALLY FILLED</t>
+  </si>
+  <si>
+    <t>EU legal reference</t>
+  </si>
+  <si>
+    <t>Res ID</t>
+  </si>
+  <si>
+    <t>EU legislation related to the reason for sampling</t>
+  </si>
+  <si>
+    <t>Prog ID</t>
+  </si>
+  <si>
+    <t>progIdSuffix</t>
+  </si>
+  <si>
+    <t>POS</t>
+  </si>
+  <si>
+    <t>AND((%anMethType.code==AT13A),(RELATION{SummarizedInformation,source.code}==F01.A057G))</t>
+  </si>
+  <si>
+    <t>IF(OR((%internalOpType.label==Reject),(%internalOpType.label==Submit)),No,Yes)</t>
+  </si>
+  <si>
+    <t>(RELATION{SummarizedInformation,source.code}==F01.A057G)</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation,source.code}</t>
+  </si>
+  <si>
+    <t>IF((%internalOpType.label!=Insert),RELATION{Report,reportDatasetId.label},)</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>MTX.gender</t>
+  </si>
+  <si>
+    <t>IF((RELATION{SummarizedInformation,type.code}==RGT),SCRAPIE,)</t>
+  </si>
+  <si>
+    <t>N123A</t>
+  </si>
+  <si>
+    <t>sexLists</t>
+  </si>
+  <si>
+    <t>FM</t>
+  </si>
+  <si>
+    <t>(RELATION{SummarizedInformation,type.code}==RGT)</t>
+  </si>
+  <si>
+    <t>%progLegalRef.code|IF_NOT_NULL(RELATION{SummarizedInformation,tseTargetGroup.code},.|RELATION{SummarizedInformation,tseTargetGroup.code},)</t>
+  </si>
+  <si>
+    <t>reportLastMessageId</t>
+  </si>
+  <si>
+    <t>reportLastModifyingMessageId</t>
+  </si>
+  <si>
+    <t>DO NOT TOUCH, used with Refresh Status/Display ack</t>
+  </si>
+  <si>
+    <t>IF((RELATION{SummarizedInformation,type.code}==CWD),RELATION{SummarizedInformation,sex.code},RELATION{CasesInformation,sex.code})</t>
+  </si>
+  <si>
+    <t>A04MQ#RELATION{SummarizedInformation,source.code}$RELATION{CasesInformation,part.code}$RELATION{SummarizedInformation,prod.code}|IF_NOT_NULL(%animage.code,$%animage.code,)|IF_NOT_NULL(%sex.code,$%sex.code,)</t>
+  </si>
+  <si>
+    <t>A04MQ#%source.code$%prod.code|IF((%type.code!=RGT),$%animage.code,)|IF_NOT_NULL(%sex.code,$%sex.code,)</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(%PSUId.label,PSUId=%PSUId.label,)</t>
+  </si>
+  <si>
+    <t>PSUId</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(RELATION{CasesInformation,animalId.code},animalId=RELATION{CasesInformation,animalId.code},)|IF_NOT_NULL(RELATION{CasesInformation,herdId.label},$herdId=RELATION{CasesInformation,herdId.label}, )|IF_NOT_NULL(RELATION{CasesInformation,sampHoldingId.label},$sampHoldingId=RELATION{CasesInformation,sampHoldingId.label},)|IF_NOT_NULL(RELATION{SummarizedInformation,PSUId.label},$PSUId=RELATION{SummarizedInformation,PSUId.label},)</t>
+  </si>
+  <si>
+    <t>Sample/case assessment</t>
+  </si>
+  <si>
+    <t>First test type</t>
+  </si>
+  <si>
+    <t>First test</t>
+  </si>
+  <si>
+    <t>Type of the first executed test</t>
+  </si>
+  <si>
+    <t>First executed test</t>
+  </si>
+  <si>
+    <t>sampInfo</t>
+  </si>
+  <si>
+    <t>D.11</t>
+  </si>
+  <si>
+    <t>origSampId</t>
+  </si>
+  <si>
+    <t>sampUnitType</t>
+  </si>
+  <si>
+    <t>C.02</t>
+  </si>
+  <si>
+    <t>G199A</t>
+  </si>
+  <si>
+    <t>H.01</t>
+  </si>
+  <si>
+    <t>anPortSeq</t>
+  </si>
+  <si>
+    <t>Portion</t>
+  </si>
+  <si>
+    <t>Portion of the analyzed sample</t>
+  </si>
+  <si>
+    <t>AND((%sampEventAsses.code!=J051A),(RELATION{SummarizedInformation,type.code}!=RGT))</t>
+  </si>
+  <si>
+    <t>sampEventAsses</t>
+  </si>
+  <si>
+    <t>AND((%sampEventAsses.code!=J051A),(RELATION{SummarizedInformation,prod.code}==F21.A07RV),(RELATION{SummarizedInformation,type.code}!=RGT))</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(RELATION{CasesInformation,tseNationalCaseId.label},tseNationalCaseId=RELATION{CasesInformation,tseNationalCaseId.label}$,)|IF_NOT_NULL(RELATION{CasesInformation,tseIndexCase.code},tseIndexCase=RELATION{CasesInformation,tseIndexCase.code}$,)|IF_NOT_NULL(RELATION{CasesInformation,sampEventAsses.code},sampEventAsses=RELATION{CasesInformation,sampEventAsses.code},)|IF_NOT_NULL(RELATION{CasesInformation,evalCom.label},$com=RELATION{CasesInformation,evalCom.label},)</t>
+  </si>
+  <si>
+    <t>cwdExtCont</t>
+  </si>
+  <si>
+    <t>pref11</t>
+  </si>
+  <si>
+    <t>yesNoLists</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Sex of the animals</t>
+  </si>
+  <si>
+    <t>%type.code|$%anMethType.code</t>
+  </si>
+  <si>
+    <t>(%type.code==SCRAPIE)</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(%statusHerd.code,statusHerd=%statusHerd.code,)</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>IF(OR((%country.code==EE),(%country.code==FI),(%country.code==LV),(%country.code==LT),(%country.code==PL),(%country.code==SE)),Y,ALL)</t>
+  </si>
+  <si>
+    <t>OR((%type.code==CWD),(%type.code==BSEOS))</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(RELATION{CasesInformation,birthCountry.code},birthCountry=RELATION{CasesInformation,birthCountry.code},)|IF_NOT_NULL(RELATION{SummarizedInformation,statusHerd.code},$statusHerd=RELATION{SummarizedInformation,statusHerd.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthInFlockHerd.code},$birthInFlockHerd=RELATION{CasesInformation,birthInFlockHerd.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthYear.code},$birthYear=RELATION{CasesInformation,birthYear.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthMonth.code},$birthMonth=RELATION{CasesInformation,birthMonth.code},)</t>
+  </si>
+  <si>
+    <t>Herd/Flock status</t>
+  </si>
+  <si>
+    <t>Husbandry system</t>
+  </si>
+  <si>
+    <t>Aggregated-Data-(Level-1)</t>
+  </si>
+  <si>
+    <t>Sample-Level-Data-(Level-2)</t>
+  </si>
+  <si>
+    <t>Analytical-Test-Results-(Level-3)</t>
+  </si>
+  <si>
+    <t>Report-Management</t>
+  </si>
+  <si>
+    <t>IF(OR((%type.code==SCRAPIE),(%type.code==BSEOS)),F,)</t>
+  </si>
+  <si>
+    <t>%progId.label|.0</t>
+  </si>
+  <si>
+    <t>%progId.label</t>
+  </si>
+  <si>
+    <t>NEXT(,)</t>
+  </si>
+  <si>
+    <t>Dataset ID</t>
+  </si>
+  <si>
+    <t>Report Status</t>
+  </si>
+  <si>
+    <t>IF((%type.code!=RGT), origSampId=%sampId.label, )</t>
+  </si>
+  <si>
+    <t>(%type.code==RGT)</t>
+  </si>
+  <si>
+    <t>F01.A057G</t>
+  </si>
+  <si>
+    <t>IF((%type.code==RGT),RF-00004629-PAR#allele=%allele1.label$allele=%allele2.label,RF-00004628-PAR)</t>
+  </si>
+  <si>
+    <t>IF((%type.code==RGT),0,)</t>
+  </si>
+  <si>
+    <t>IF(OR((%type.code!=CWD),(RELATION{Preferences,cwdExtCont.code}==N)),F32.A0C9B,)</t>
+  </si>
+  <si>
+    <t>(RELATION{SummarizedInformation,sex.code}==F32.A0C9B)</t>
+  </si>
+  <si>
+    <t>IF((RELATION{SummarizedInformation,sex.code}!=F32.A0C9B),RELATION{SummarizedInformation,sex.code},)</t>
+  </si>
+  <si>
+    <t>IF((%type.code==RGT),F01.A057G,)IF((%type.code==BSE),F01.A057E,)IF(AND((%type.code==CWD),(RELATION{Preferences,cwdExtCont.code}==N)),F01.A056M,)</t>
+  </si>
+  <si>
+    <t>AND((%type.code==CWD),(RELATION{Preferences,cwdExtCont.code}==Y))</t>
+  </si>
+  <si>
+    <t>(%type.code==CWD)</t>
+  </si>
+  <si>
+    <t>IF((%type.code!=RGT),tseTargetGroup=%tseTargetGroup.code$totSamplesTested=%totSamplesTested.label$totSamplesPositive=%totSamplesPositive.label$totSamplesNegative=%totSamplesNegative.label$totSamplesInconclusive=%totSamplesInconclusive.label$totSamplesUnsuitable=%totSamplesUnsuitable.label,totSamplesTested=%totSamplesTested.label)</t>
+  </si>
+  <si>
+    <t>IF((%type.code!=RGT),SUM(%totSamplesPositive.label,%totSamplesNegative.label,%totSamplesInconclusive.label),)</t>
+  </si>
+  <si>
+    <t>PSU id required</t>
+  </si>
+  <si>
+    <t>Flag to include Primary Sample Unit as mandatory field</t>
+  </si>
+  <si>
+    <t>IF((%type.code==RGT),F01.A057G,)IF((%type.code==BSE),F01.A057E,)</t>
+  </si>
+  <si>
+    <t>(%sampEventAsses.code!=J051A)</t>
+  </si>
+  <si>
+    <t>IF((%type.code==RGT),AT13A,AT06A)</t>
+  </si>
+  <si>
+    <t>IF((%type.code==SCRAPIE),RELATION{Preferences,defScreeningSCRAPIE.code},)IF((%type.code==CWD),RELATION{Preferences,defScreeningCWD.code},)IF(OR((%type.code==BSE),(%type.code==BSEOS)),RELATION{Preferences,defScreeningBSE.code},)IF((%type.code==RGT),F089A,)</t>
+  </si>
+  <si>
+    <t>SCRAPIE$AT06A</t>
+  </si>
+  <si>
+    <t>IF((%type.code==SCRAPIE),BSE,%type.code)</t>
+  </si>
+  <si>
+    <t>origSampId=%origSampId.label</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation,animage.code}</t>
+  </si>
+  <si>
+    <t>%paramCodeBaseTerm.code</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation,progId.label}|.%progIdSuffix.code</t>
+  </si>
+  <si>
     <t>RELATION{SummarizedInformation,type.code}$%anMethType.code</t>
   </si>
   <si>
-    <t>RELATION{SummarizedInformation,progId.label}|.|ZERO_PADDING({rowId},6)</t>
-  </si>
-  <si>
-    <t>%country.code|END_TRIM(%reportYear.code,2)|END_TRIM(ZERO_PADDING(%reportMonth.code,2),2)</t>
-  </si>
-  <si>
-    <t>RELATION{Report,reportSenderId.label}|IF_NOT_NULL(RELATION{Report,reportVersion.code},.RELATION{Report,reportVersion.code},)</t>
-  </si>
-  <si>
-    <t>Born in the flock</t>
-  </si>
-  <si>
-    <t>Number of Negative Animals</t>
-  </si>
-  <si>
-    <t>Total number of Tested Samples/Animals</t>
-  </si>
-  <si>
-    <t>Executed test</t>
-  </si>
-  <si>
-    <t>IF((%type.code==RGT),,0)</t>
-  </si>
-  <si>
-    <t>(%type.code!=RGT)</t>
-  </si>
-  <si>
-    <t>RELATION{SummarizedInformation,progId.label}|.IF_NOT_NULL(RELATION{CasesInformation,animalId.label},A.|RELATION{CasesInformation,animalId.label},S.|RELATION{CasesInformation,sampId.label})</t>
-  </si>
-  <si>
-    <t>(RELATION{SummarizedInformation,type.code}!=RGT)</t>
-  </si>
-  <si>
-    <t>IF_NOT_NULL(RELATION{SummarizedInformation,tseTargetGroup.code},tseTargetGroup=RELATION{SummarizedInformation,tseTargetGroup.code},)</t>
-  </si>
-  <si>
-    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT),F02.A06AM,F02.A06AL)</t>
-  </si>
-  <si>
-    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT),Brain,Blood)</t>
-  </si>
-  <si>
-    <t>reportYearsList</t>
-  </si>
-  <si>
-    <t>animalYearsList</t>
-  </si>
-  <si>
-    <t>reportPreviousStatus</t>
-  </si>
-  <si>
-    <t>repPreviousStatus</t>
-  </si>
-  <si>
-    <t>DO NOT TOUCH, AUTOMATICALLY FILLED</t>
-  </si>
-  <si>
-    <t>EU legal reference</t>
-  </si>
-  <si>
-    <t>Res ID</t>
-  </si>
-  <si>
-    <t>EU legislation related to the reason for sampling</t>
-  </si>
-  <si>
-    <t>Prog ID</t>
-  </si>
-  <si>
-    <t>progIdSuffix</t>
-  </si>
-  <si>
-    <t>POS</t>
-  </si>
-  <si>
-    <t>AND((%anMethType.code==AT13A),(RELATION{SummarizedInformation,source.code}==F01.A057G))</t>
-  </si>
-  <si>
-    <t>IF(OR((%internalOpType.label==Reject),(%internalOpType.label==Submit)),No,Yes)</t>
-  </si>
-  <si>
-    <t>(RELATION{SummarizedInformation,source.code}==F01.A057G)</t>
-  </si>
-  <si>
-    <t>RELATION{SummarizedInformation,source.code}</t>
-  </si>
-  <si>
-    <t>IF((%internalOpType.label!=Insert),RELATION{Report,reportDatasetId.label},)</t>
-  </si>
-  <si>
-    <t>sex</t>
-  </si>
-  <si>
-    <t>MTX.gender</t>
-  </si>
-  <si>
-    <t>IF((RELATION{SummarizedInformation,type.code}==RGT),SCRAPIE,)</t>
-  </si>
-  <si>
-    <t>N123A</t>
-  </si>
-  <si>
-    <t>sexLists</t>
-  </si>
-  <si>
-    <t>FM</t>
-  </si>
-  <si>
-    <t>(RELATION{SummarizedInformation,type.code}==RGT)</t>
-  </si>
-  <si>
-    <t>%progLegalRef.code|IF_NOT_NULL(RELATION{SummarizedInformation,tseTargetGroup.code},.|RELATION{SummarizedInformation,tseTargetGroup.code},)</t>
-  </si>
-  <si>
-    <t>RELATION{SummarizedInformation,progId.label}|IF((RELATION{SummarizedInformation,type.code}!=RGT),.%progIdSuffix.code,)</t>
-  </si>
-  <si>
-    <t>reportLastMessageId</t>
-  </si>
-  <si>
-    <t>reportLastModifyingMessageId</t>
-  </si>
-  <si>
-    <t>DO NOT TOUCH, used with Refresh Status/Display ack</t>
-  </si>
-  <si>
-    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT),RELATION{SummarizedInformation,animage.code},RELATION{CasesInformation,animage.code})</t>
-  </si>
-  <si>
-    <t>IF((RELATION{SummarizedInformation,type.code}==CWD),RELATION{SummarizedInformation,sex.code},RELATION{CasesInformation,sex.code})</t>
-  </si>
-  <si>
-    <t>A04MQ#RELATION{SummarizedInformation,source.code}$RELATION{CasesInformation,part.code}$RELATION{SummarizedInformation,prod.code}|IF_NOT_NULL(%animage.code,$%animage.code,)|IF_NOT_NULL(%sex.code,$%sex.code,)</t>
-  </si>
-  <si>
-    <t>A04MQ#%source.code$%prod.code|IF((%type.code!=RGT),$%animage.code,)|IF_NOT_NULL(%sex.code,$%sex.code,)</t>
-  </si>
-  <si>
-    <t>IF_NOT_NULL(%PSUId.label,PSUId=%PSUId.label,)</t>
-  </si>
-  <si>
-    <t>PSUId</t>
-  </si>
-  <si>
-    <t>IF_NOT_NULL(RELATION{CasesInformation,animalId.code},animalId=RELATION{CasesInformation,animalId.code},)|IF_NOT_NULL(RELATION{CasesInformation,herdId.label},$herdId=RELATION{CasesInformation,herdId.label}, )|IF_NOT_NULL(RELATION{CasesInformation,sampHoldingId.label},$sampHoldingId=RELATION{CasesInformation,sampHoldingId.label},)|IF_NOT_NULL(RELATION{SummarizedInformation,PSUId.label},$PSUId=RELATION{SummarizedInformation,PSUId.label},)</t>
-  </si>
-  <si>
-    <t>Sample/case assessment</t>
-  </si>
-  <si>
-    <t>First test type</t>
-  </si>
-  <si>
-    <t>First test</t>
-  </si>
-  <si>
-    <t>Type of the first executed test</t>
-  </si>
-  <si>
-    <t>First executed test</t>
-  </si>
-  <si>
-    <t>sampInfo</t>
-  </si>
-  <si>
-    <t>D.11</t>
-  </si>
-  <si>
-    <t>origSampId</t>
-  </si>
-  <si>
-    <t>sampUnitType</t>
-  </si>
-  <si>
-    <t>C.02</t>
-  </si>
-  <si>
-    <t>G199A</t>
-  </si>
-  <si>
-    <t>H.01</t>
-  </si>
-  <si>
-    <t>anPortSeq</t>
-  </si>
-  <si>
-    <t>Portion</t>
-  </si>
-  <si>
-    <t>Portion of the analyzed sample</t>
-  </si>
-  <si>
-    <t>AND((%sampEventAsses.code!=J051A),(RELATION{SummarizedInformation,type.code}!=RGT))</t>
-  </si>
-  <si>
-    <t>sampEventAsses</t>
-  </si>
-  <si>
-    <t>AND((%sampEventAsses.code!=J051A),(RELATION{SummarizedInformation,prod.code}==F21.A07RV),(RELATION{SummarizedInformation,type.code}!=RGT))</t>
-  </si>
-  <si>
-    <t>IF_NOT_NULL(RELATION{CasesInformation,tseNationalCaseId.label},tseNationalCaseId=RELATION{CasesInformation,tseNationalCaseId.label}$,)|IF_NOT_NULL(RELATION{CasesInformation,tseIndexCase.code},tseIndexCase=RELATION{CasesInformation,tseIndexCase.code}$,)|IF_NOT_NULL(RELATION{CasesInformation,sampEventAsses.code},sampEventAsses=RELATION{CasesInformation,sampEventAsses.code},)|IF_NOT_NULL(RELATION{CasesInformation,evalCom.label},$com=RELATION{CasesInformation,evalCom.label},)</t>
-  </si>
-  <si>
-    <t>cwdExtCont</t>
-  </si>
-  <si>
-    <t>pref11</t>
-  </si>
-  <si>
-    <t>yesNoLists</t>
-  </si>
-  <si>
-    <t>ALL</t>
-  </si>
-  <si>
-    <t>Sex</t>
-  </si>
-  <si>
-    <t>Sex of the animals</t>
-  </si>
-  <si>
-    <t>%type.code|$%anMethType.code</t>
-  </si>
-  <si>
-    <t>(%type.code==SCRAPIE)</t>
-  </si>
-  <si>
-    <t>IF_NOT_NULL(%statusHerd.code,statusHerd=%statusHerd.code,)</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>IF(OR((%country.code==EE),(%country.code==FI),(%country.code==LV),(%country.code==LT),(%country.code==PL),(%country.code==SE)),Y,ALL)</t>
-  </si>
-  <si>
-    <t>OR((%type.code==CWD),(%type.code==BSEOS))</t>
-  </si>
-  <si>
-    <t>IF_NOT_NULL(RELATION{CasesInformation,birthCountry.code},birthCountry=RELATION{CasesInformation,birthCountry.code},)|IF_NOT_NULL(RELATION{SummarizedInformation,statusHerd.code},$statusHerd=RELATION{SummarizedInformation,statusHerd.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthInFlockHerd.code},$birthInFlockHerd=RELATION{CasesInformation,birthInFlockHerd.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthYear.code},$birthYear=RELATION{CasesInformation,birthYear.code},)|IF_NOT_NULL(RELATION{CasesInformation,birthMonth.code},$birthMonth=RELATION{CasesInformation,birthMonth.code},)</t>
-  </si>
-  <si>
-    <t>Herd/Flock status</t>
-  </si>
-  <si>
-    <t>Husbandry system</t>
-  </si>
-  <si>
-    <t>Aggregated-Data-(Level-1)</t>
-  </si>
-  <si>
-    <t>Sample-Level-Data-(Level-2)</t>
-  </si>
-  <si>
-    <t>Analytical-Test-Results-(Level-3)</t>
-  </si>
-  <si>
-    <t>Report-Management</t>
-  </si>
-  <si>
-    <t>IF(OR((%type.code==SCRAPIE),(%type.code==BSEOS)),F,)</t>
-  </si>
-  <si>
-    <t>%progId.label|.0</t>
-  </si>
-  <si>
-    <t>%progId.label</t>
-  </si>
-  <si>
-    <t>NEXT(,)</t>
-  </si>
-  <si>
-    <t>Dataset ID</t>
-  </si>
-  <si>
-    <t>Report Status</t>
-  </si>
-  <si>
-    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT), RELATION{SummarizedInformation,sampId.label}, )</t>
-  </si>
-  <si>
-    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT), origSampId=%origSampId.label, )</t>
-  </si>
-  <si>
-    <t>IF((%type.code!=RGT), origSampId=%sampId.label, )</t>
-  </si>
-  <si>
-    <t>(%type.code==RGT)</t>
-  </si>
-  <si>
-    <t>F01.A057G</t>
-  </si>
-  <si>
-    <t>IF((%type.code==RGT),RF-00004629-PAR#allele=%allele1.label$allele=%allele2.label,RF-00004628-PAR)</t>
-  </si>
-  <si>
-    <t>IF((%type.code==RGT),0,)</t>
-  </si>
-  <si>
-    <t>IF(OR((%type.code!=CWD),(RELATION{Preferences,cwdExtCont.code}==N)),F32.A0C9B,)</t>
-  </si>
-  <si>
-    <t>(RELATION{SummarizedInformation,sex.code}==F32.A0C9B)</t>
-  </si>
-  <si>
-    <t>IF((RELATION{SummarizedInformation,sex.code}!=F32.A0C9B),RELATION{SummarizedInformation,sex.code},)</t>
-  </si>
-  <si>
-    <t>IF((%type.code==RGT),F01.A057G,)IF((%type.code==BSE),F01.A057E,)IF(AND((%type.code==CWD),(RELATION{Preferences,cwdExtCont.code}==N)),F01.A056M,)</t>
-  </si>
-  <si>
-    <t>AND((%type.code==CWD),(RELATION{Preferences,cwdExtCont.code}==Y))</t>
-  </si>
-  <si>
-    <t>(%type.code==CWD)</t>
-  </si>
-  <si>
-    <t>IF((%type.code!=RGT),tseTargetGroup=%tseTargetGroup.code$totSamplesTested=%totSamplesTested.label$totSamplesPositive=%totSamplesPositive.label$totSamplesNegative=%totSamplesNegative.label$totSamplesInconclusive=%totSamplesInconclusive.label$totSamplesUnsuitable=%totSamplesUnsuitable.label,totSamplesTested=%totSamplesTested.label)</t>
-  </si>
-  <si>
-    <t>IF((%type.code!=RGT),SUM(%totSamplesPositive.label,%totSamplesNegative.label,%totSamplesInconclusive.label),)</t>
-  </si>
-  <si>
-    <t>PSU id required</t>
-  </si>
-  <si>
-    <t>Flag to include Primary Sample Unit as mandatory field</t>
-  </si>
-  <si>
-    <t>IF((%type.code==RGT),F01.A057G,)IF((%type.code==BSE),F01.A057E,)</t>
-  </si>
-  <si>
-    <t>(%sampEventAsses.code!=J051A)</t>
-  </si>
-  <si>
-    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT),%paramCodeBaseTerm.code,RF-00004629-PAR)</t>
-  </si>
-  <si>
-    <t>IF((%type.code==RGT),AT13A,AT06A)</t>
-  </si>
-  <si>
-    <t>IF((%type.code==SCRAPIE),RELATION{Preferences,defScreeningSCRAPIE.code},)IF((%type.code==CWD),RELATION{Preferences,defScreeningCWD.code},)IF(OR((%type.code==BSE),(%type.code==BSEOS)),RELATION{Preferences,defScreeningBSE.code},)IF((%type.code==RGT),F089A,)</t>
-  </si>
-  <si>
-    <t>SCRAPIE$AT06A</t>
-  </si>
-  <si>
-    <t>IF((%type.code==SCRAPIE),BSE,%type.code)</t>
+    <t>RELATION{SummarizedInformation,sampId.label}</t>
+  </si>
+  <si>
+    <t>RELATION{SummarizedInformation,type.code}%anMethType.code</t>
   </si>
 </sst>
 </file>
@@ -3445,9 +3445,6 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table25711" displayName="Table25711" ref="A1:R43" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="A1:R43"/>
-  <sortState ref="A2:R43">
-    <sortCondition ref="A1:A43"/>
-  </sortState>
   <tableColumns count="18">
     <tableColumn id="1" name="id" dataDxfId="37"/>
     <tableColumn id="2" name="code" dataDxfId="36"/>
@@ -4153,16 +4150,16 @@
     </row>
     <row r="3" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="F3" s="24" t="s">
         <v>12</v>
@@ -4180,16 +4177,16 @@
         <v>9</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="L3" s="25" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>9</v>
@@ -4233,7 +4230,7 @@
         <v>112</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="R4" s="2">
         <v>3</v>
@@ -4271,7 +4268,7 @@
         <v>112</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="R5" s="2">
         <v>4</v>
@@ -4309,7 +4306,7 @@
         <v>112</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="R6" s="2">
         <v>5</v>
@@ -4347,7 +4344,7 @@
         <v>112</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="R7" s="2">
         <v>6</v>
@@ -4385,7 +4382,7 @@
         <v>112</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="R8" s="2">
         <v>7</v>
@@ -4423,7 +4420,7 @@
         <v>112</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="R9" s="2">
         <v>8</v>
@@ -4462,7 +4459,7 @@
         <v>112</v>
       </c>
       <c r="L10" s="27" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="R10" s="2">
         <v>9</v>
@@ -4501,7 +4498,7 @@
         <v>112</v>
       </c>
       <c r="L11" s="27" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="R11" s="2">
         <v>10</v>
@@ -4540,7 +4537,7 @@
         <v>112</v>
       </c>
       <c r="L12" s="27" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
@@ -4681,7 +4678,7 @@
         <v>9</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="8" t="s">
@@ -4786,7 +4783,7 @@
         <v>300</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>5</v>
@@ -4912,7 +4909,7 @@
       <c r="C8" s="17"/>
       <c r="D8" s="18"/>
       <c r="E8" s="17" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="F8" s="17" t="s">
         <v>174</v>
@@ -4943,13 +4940,13 @@
     </row>
     <row r="9" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
       <c r="D9" s="18"/>
       <c r="E9" s="17" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>174</v>
@@ -4980,13 +4977,13 @@
     </row>
     <row r="10" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="18"/>
       <c r="E10" s="17" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>174</v>
@@ -5024,10 +5021,10 @@
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="18" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>174</v>
@@ -5067,10 +5064,10 @@
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="18" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="F12" s="17" t="s">
         <v>174</v>
@@ -5103,15 +5100,15 @@
     </row>
     <row r="13" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="18"/>
       <c r="E13" s="17" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="F13" s="17" t="s">
         <v>174</v>
@@ -5153,11 +5150,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="M14" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="M23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M23" sqref="M23"/>
+      <selection pane="bottomRight" activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5306,7 +5303,7 @@
         <v>3</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>3</v>
@@ -5318,10 +5315,10 @@
         <v>312</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>5</v>
@@ -5341,7 +5338,7 @@
         <v>57</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>69</v>
@@ -5356,7 +5353,7 @@
         <v>3</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>3</v>
@@ -5400,10 +5397,10 @@
         <v>74</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>3</v>
@@ -5444,10 +5441,10 @@
         <v>18</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>3</v>
@@ -5470,40 +5467,40 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>3</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="L7" s="29" t="s">
         <v>312</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="P7"/>
       <c r="Q7" s="6" t="s">
@@ -5527,10 +5524,10 @@
         <v>89</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>12</v>
@@ -5539,10 +5536,10 @@
         <v>90</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>3</v>
@@ -5551,10 +5548,13 @@
         <v>308</v>
       </c>
       <c r="L8" s="29" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>471</v>
+        <v>464</v>
+      </c>
+      <c r="N8" s="33" t="s">
+        <v>464</v>
       </c>
       <c r="Q8" s="6" t="s">
         <v>9</v>
@@ -5577,10 +5577,10 @@
         <v>92</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>12</v>
@@ -5589,10 +5589,10 @@
         <v>93</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>3</v>
@@ -5601,10 +5601,13 @@
         <v>112</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>472</v>
+        <v>465</v>
+      </c>
+      <c r="N9" s="33" t="s">
+        <v>465</v>
       </c>
       <c r="Q9" s="6" t="s">
         <v>9</v>
@@ -5624,7 +5627,7 @@
         <v>34</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>36</v>
@@ -5636,10 +5639,10 @@
         <v>37</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>3</v>
@@ -5651,7 +5654,10 @@
         <v>312</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>445</v>
+        <v>441</v>
+      </c>
+      <c r="N10" s="33" t="s">
+        <v>441</v>
       </c>
       <c r="Q10" s="6" t="s">
         <v>5</v>
@@ -5665,23 +5671,23 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>202</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>174</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="6" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>3</v>
@@ -5707,7 +5713,7 @@
         <v>25</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F12" s="21" t="s">
         <v>238</v>
@@ -5716,16 +5722,16 @@
         <v>8</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O12" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="Q12" s="6" t="s">
         <v>5</v>
@@ -5754,16 +5760,16 @@
         <v>8</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O13" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="Q13" s="6" t="s">
         <v>5</v>
@@ -5792,16 +5798,16 @@
         <v>8</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="J14" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O14" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="Q14" s="6" t="s">
         <v>5</v>
@@ -5821,7 +5827,7 @@
         <v>20</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>238</v>
@@ -5830,19 +5836,19 @@
         <v>8</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O15" s="6" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="P15" s="6" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="Q15" s="6" t="s">
         <v>5</v>
@@ -5871,16 +5877,16 @@
         <v>8</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>3</v>
       </c>
       <c r="O16" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="Q16" s="6" t="s">
         <v>5</v>
@@ -5900,7 +5906,7 @@
         <v>7</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F17" s="17" t="s">
         <v>174</v>
@@ -5918,7 +5924,7 @@
         <v>3</v>
       </c>
       <c r="O17" s="6" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>9</v>
@@ -5945,10 +5951,10 @@
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="6" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>3</v>
@@ -5957,7 +5963,7 @@
         <v>319</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="Q18" s="6" t="s">
         <v>5</v>
@@ -5987,10 +5993,10 @@
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="6" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="J19" s="6" t="s">
         <v>3</v>
@@ -5999,7 +6005,7 @@
         <v>319</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="Q19" s="6" t="s">
         <v>5</v>
@@ -6077,10 +6083,10 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>346</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>347</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>174</v>
@@ -6128,7 +6134,7 @@
       </c>
       <c r="M23" s="33"/>
       <c r="P23" s="6" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="Q23" s="6" t="s">
         <v>9</v>
@@ -6215,7 +6221,7 @@
         <v>4</v>
       </c>
       <c r="P26" s="6" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="Q26" s="6" t="s">
         <v>9</v>
@@ -6244,7 +6250,7 @@
         <v>4</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="Q27" s="6" t="s">
         <v>3</v>
@@ -6366,7 +6372,7 @@
         <v>4</v>
       </c>
       <c r="P31" s="6" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="Q31" s="6" t="s">
         <v>9</v>
@@ -6398,7 +6404,7 @@
         <v>4</v>
       </c>
       <c r="P32" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="Q32" s="6" t="s">
         <v>9</v>
@@ -6462,7 +6468,7 @@
         <v>4</v>
       </c>
       <c r="P34" s="6" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="Q34" s="6" t="s">
         <v>9</v>
@@ -6494,7 +6500,7 @@
         <v>4</v>
       </c>
       <c r="P35" s="6" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="Q35" s="6" t="s">
         <v>9</v>
@@ -6502,13 +6508,13 @@
     </row>
     <row r="36" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>174</v>
@@ -6523,7 +6529,7 @@
         <v>4</v>
       </c>
       <c r="P36" s="6" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="Q36" s="6" t="s">
         <v>9</v>
@@ -6590,7 +6596,7 @@
         <v>4</v>
       </c>
       <c r="P38" s="6" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="Q38" s="6" t="s">
         <v>9</v>
@@ -6651,7 +6657,7 @@
         <v>4</v>
       </c>
       <c r="P40" s="6" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="Q40" s="6" t="s">
         <v>9</v>
@@ -6730,7 +6736,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M6" sqref="M6"/>
+      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6817,13 +6823,13 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B2" t="s">
         <v>191</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>211</v>
@@ -6835,10 +6841,10 @@
         <v>320</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="J2" s="30" t="s">
         <v>3</v>
@@ -6926,10 +6932,10 @@
         <v>303</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>5</v>
@@ -6943,40 +6949,40 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="Q5" s="6" t="s">
         <v>5</v>
@@ -7005,10 +7011,10 @@
         <v>74</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="J6" s="30" t="s">
         <v>4</v>
@@ -7017,7 +7023,7 @@
         <v>111</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="Q6" s="6" t="s">
         <v>5</v>
@@ -7046,7 +7052,7 @@
         <v>8</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>3</v>
@@ -7084,7 +7090,7 @@
         <v>8</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>3</v>
@@ -7228,7 +7234,7 @@
         <v>217</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="I12" s="17" t="s">
         <v>3</v>
@@ -7269,13 +7275,13 @@
         <v>197</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="I13" s="29" t="s">
         <v>3</v>
       </c>
       <c r="J13" s="30" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>198</v>
@@ -7312,7 +7318,7 @@
         <v>42</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="I14" s="17" t="s">
         <v>3</v>
@@ -7352,7 +7358,7 @@
         <v>282</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>3</v>
@@ -7361,7 +7367,7 @@
         <v>3</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="Q15" s="6" t="s">
         <v>5</v>
@@ -7388,7 +7394,7 @@
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="6" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="I16" s="20" t="s">
         <v>3</v>
@@ -7414,7 +7420,7 @@
         <v>34</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>309</v>
@@ -7435,10 +7441,10 @@
         <v>3</v>
       </c>
       <c r="K17" s="20" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>5</v>
@@ -7559,10 +7565,10 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>346</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>347</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>174</v>
@@ -7597,11 +7603,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="M8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="K35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M14" sqref="M14"/>
+      <selection pane="bottomRight" activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7698,19 +7704,19 @@
         <v>12</v>
       </c>
       <c r="H2" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>383</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>383</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>385</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>319</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="Q2" s="6" t="s">
         <v>5</v>
@@ -7736,19 +7742,19 @@
         <v>12</v>
       </c>
       <c r="H3" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>383</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>383</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>385</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>319</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>5</v>
@@ -7789,7 +7795,7 @@
         <v>3</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="M4" s="6" t="s">
         <v>294</v>
@@ -7824,7 +7830,7 @@
         <v>4</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>400</v>
+        <v>469</v>
       </c>
       <c r="Q5" s="6" t="s">
         <v>5</v>
@@ -7844,7 +7850,7 @@
         <v>142</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>12</v>
@@ -7864,8 +7870,8 @@
       <c r="K6" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="L6" s="6" t="s">
-        <v>357</v>
+      <c r="L6" s="33" t="s">
+        <v>472</v>
       </c>
       <c r="Q6" s="6" t="s">
         <v>9</v>
@@ -7958,19 +7964,19 @@
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>174</v>
@@ -8037,7 +8043,7 @@
         <v>4</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="Q11" s="6" t="s">
         <v>9</v>
@@ -8045,10 +8051,10 @@
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>174</v>
@@ -8063,7 +8069,7 @@
         <v>4</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>451</v>
+        <v>473</v>
       </c>
       <c r="Q12" s="6" t="s">
         <v>5</v>
@@ -8188,7 +8194,7 @@
         <v>4</v>
       </c>
       <c r="P16" s="6" t="s">
-        <v>396</v>
+        <v>471</v>
       </c>
       <c r="Q16" s="6" t="s">
         <v>9</v>
@@ -8196,7 +8202,7 @@
     </row>
     <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>174</v>
@@ -8214,7 +8220,7 @@
         <v>4</v>
       </c>
       <c r="P17" s="6" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>5</v>
@@ -8246,7 +8252,7 @@
         <v>4</v>
       </c>
       <c r="P18" s="6" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="Q18" s="6" t="s">
         <v>9</v>
@@ -8263,10 +8269,10 @@
         <v>11</v>
       </c>
       <c r="D19" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>377</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>379</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>174</v>
@@ -8284,7 +8290,7 @@
         <v>4</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="Q19" s="6" t="s">
         <v>9</v>
@@ -8385,7 +8391,7 @@
         <v>95</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>256</v>
@@ -8406,7 +8412,7 @@
         <v>3</v>
       </c>
       <c r="O23" s="6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="Q23" s="6" t="s">
         <v>9</v>
@@ -8441,7 +8447,7 @@
         <v>4</v>
       </c>
       <c r="M24" s="6" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="Q24" s="6" t="s">
         <v>9</v>
@@ -8633,7 +8639,7 @@
         <v>4</v>
       </c>
       <c r="P30" s="6" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="Q30" s="6" t="s">
         <v>9</v>
@@ -8662,7 +8668,7 @@
         <v>4</v>
       </c>
       <c r="P31" s="6" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="Q31" s="6" t="s">
         <v>9</v>
@@ -8708,13 +8714,13 @@
     </row>
     <row r="33" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>174</v>
@@ -8729,7 +8735,7 @@
         <v>4</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>452</v>
+        <v>468</v>
       </c>
       <c r="Q33" s="6" t="s">
         <v>9</v>
@@ -8793,7 +8799,7 @@
         <v>4</v>
       </c>
       <c r="P35" s="6" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q35" s="6" t="s">
         <v>9</v>
@@ -8889,7 +8895,7 @@
         <v>4</v>
       </c>
       <c r="P38" s="6" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="Q38" s="6" t="s">
         <v>9</v>
@@ -8897,13 +8903,13 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>174</v>
@@ -8918,13 +8924,13 @@
         <v>4</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="N39" s="6" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="O39" s="6" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="Q39" s="6" t="s">
         <v>9</v>
@@ -8967,7 +8973,7 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>57</v>
@@ -8985,7 +8991,7 @@
         <v>4</v>
       </c>
       <c r="N41" s="6" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="Q41" s="6" t="s">
         <v>5</v>
@@ -9025,19 +9031,19 @@
         <v>85</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>368</v>
+        <v>3</v>
       </c>
       <c r="K43" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="L43" s="6" t="s">
-        <v>341</v>
+      <c r="L43" s="33" t="s">
+        <v>474</v>
       </c>
       <c r="Q43" s="6" t="s">
         <v>5</v>
@@ -9235,7 +9241,7 @@
         <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -9243,7 +9249,7 @@
         <v>170</v>
       </c>
       <c r="B3" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -9267,7 +9273,7 @@
         <v>221</v>
       </c>
       <c r="B6" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -9275,7 +9281,7 @@
         <v>227</v>
       </c>
       <c r="B7" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
   </sheetData>
@@ -9474,7 +9480,7 @@
       <c r="L4" s="2"/>
       <c r="M4" s="6"/>
       <c r="P4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>3</v>
@@ -9580,7 +9586,7 @@
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="Q8" s="2" t="s">
         <v>3</v>
@@ -9639,10 +9645,10 @@
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
       <c r="P10" s="4" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
@@ -9698,15 +9704,15 @@
         <v>4</v>
       </c>
       <c r="P12" s="10" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="13" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E13" s="22" t="s">
         <v>315</v>

</xml_diff>